<commit_message>
Más cosas en el excel de preguntas y respuestas
</commit_message>
<xml_diff>
--- a/Preguntas y respuestas.xlsx
+++ b/Preguntas y respuestas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\Facultad 2019\Algoritmos y estructura de datos\TP 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\Facultad 2019\Algoritmos y estructura de datos\TP 2019\Repositorio\TPAlgoritmos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22F5028-1E7B-44B9-9E15-47590DB633B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56771B6-702F-49C5-AEA3-CD5AF7B492A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{568DC9B8-9665-4EC8-9CD9-1389A254C195}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="161">
   <si>
     <t>Categoría</t>
   </si>
@@ -421,6 +421,99 @@
   </si>
   <si>
     <t>D-Río Congo</t>
+  </si>
+  <si>
+    <t>Ciencia</t>
+  </si>
+  <si>
+    <t>¿Cómo se llama el proceso por el cual una célula se divide para formar dos células hijas?</t>
+  </si>
+  <si>
+    <t>A-Segregación</t>
+  </si>
+  <si>
+    <t>B-Mitosis</t>
+  </si>
+  <si>
+    <t>C-Meiosis</t>
+  </si>
+  <si>
+    <t>D-Fotosíntesis</t>
+  </si>
+  <si>
+    <t>¿Cuál es la función principal de los globulos rojos?</t>
+  </si>
+  <si>
+    <t>A-Combatir enfermedades</t>
+  </si>
+  <si>
+    <t>B-Coagular la sangre</t>
+  </si>
+  <si>
+    <t>C-Llevar oxígeno</t>
+  </si>
+  <si>
+    <t>D-Producir anticuerpos</t>
+  </si>
+  <si>
+    <t>¿Cuál es la velocidad a la que viaja la luz?</t>
+  </si>
+  <si>
+    <t>A-300.000 m/s</t>
+  </si>
+  <si>
+    <t>B-300.000 km/s</t>
+  </si>
+  <si>
+    <t>C-30.000 km/h</t>
+  </si>
+  <si>
+    <t>D-300.000km/h</t>
+  </si>
+  <si>
+    <t>¿Cuál es la fuerza física que la Tierra ejerce sobre los cuerpos hacia su centro?</t>
+  </si>
+  <si>
+    <t>A-Gravedad</t>
+  </si>
+  <si>
+    <t>B-Normal</t>
+  </si>
+  <si>
+    <t>C-Rozamiento</t>
+  </si>
+  <si>
+    <t>D-Atracción</t>
+  </si>
+  <si>
+    <t>¿Dónde se localiza la información genética en las células?</t>
+  </si>
+  <si>
+    <t>A-En el núcleo</t>
+  </si>
+  <si>
+    <t>B-En la membrana</t>
+  </si>
+  <si>
+    <t>C-En el citoplasma</t>
+  </si>
+  <si>
+    <t>D-Ribosoma</t>
+  </si>
+  <si>
+    <t>¿Cómo se llaman las partículas subatómicas con carga eléctrica negativa?</t>
+  </si>
+  <si>
+    <t>A-Neutrones</t>
+  </si>
+  <si>
+    <t>B-Protones</t>
+  </si>
+  <si>
+    <t>C-Electrones</t>
+  </si>
+  <si>
+    <t>D-Átomos</t>
   </si>
 </sst>
 </file>
@@ -482,10 +575,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -804,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC6222F-3F2B-43BB-8383-758C7F06C17A}">
   <dimension ref="A1:X161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,10 +941,10 @@
       <c r="W1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -880,9 +973,9 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
         <v>84</v>
       </c>
@@ -909,9 +1002,9 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+    <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="2" t="s">
         <v>85</v>
       </c>
@@ -938,9 +1031,9 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
         <v>86</v>
       </c>
@@ -968,10 +1061,10 @@
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1001,8 +1094,8 @@
       <c r="W6" s="3"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
         <v>88</v>
       </c>
@@ -1030,8 +1123,8 @@
       <c r="W7" s="3"/>
     </row>
     <row r="8" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
         <v>89</v>
       </c>
@@ -1059,8 +1152,8 @@
       <c r="W8" s="3"/>
     </row>
     <row r="9" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
         <v>90</v>
       </c>
@@ -1088,10 +1181,10 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1121,8 +1214,8 @@
       <c r="W10" s="3"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
         <v>92</v>
       </c>
@@ -1150,8 +1243,8 @@
       <c r="W11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
         <v>93</v>
       </c>
@@ -1179,8 +1272,8 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="2" t="s">
         <v>94</v>
       </c>
@@ -1208,10 +1301,10 @@
       <c r="W13" s="3"/>
     </row>
     <row r="14" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1240,9 +1333,9 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+    <row r="15" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="2" t="s">
         <v>96</v>
       </c>
@@ -1269,9 +1362,9 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+    <row r="16" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="2" t="s">
         <v>97</v>
       </c>
@@ -1298,9 +1391,9 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+    <row r="17" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
         <v>98</v>
       </c>
@@ -1328,10 +1421,10 @@
       <c r="W17" s="3"/>
     </row>
     <row r="18" spans="1:23" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1360,9 +1453,9 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+    <row r="19" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>100</v>
       </c>
@@ -1390,8 +1483,8 @@
       <c r="W19" s="3"/>
     </row>
     <row r="20" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="2" t="s">
         <v>101</v>
       </c>
@@ -1418,9 +1511,9 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+    <row r="21" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="2" t="s">
         <v>102</v>
       </c>
@@ -1448,10 +1541,10 @@
       <c r="W21" s="3"/>
     </row>
     <row r="22" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1480,9 +1573,9 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" ht="63" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+    <row r="23" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
         <v>104</v>
       </c>
@@ -1509,9 +1602,9 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+    <row r="24" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="2" t="s">
         <v>105</v>
       </c>
@@ -1538,9 +1631,9 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+    <row r="25" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="2" t="s">
         <v>106</v>
       </c>
@@ -1568,10 +1661,10 @@
       <c r="W25" s="3"/>
     </row>
     <row r="26" spans="1:23" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1601,8 +1694,8 @@
       <c r="W26" s="3"/>
     </row>
     <row r="27" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="2" t="s">
         <v>108</v>
       </c>
@@ -1630,8 +1723,8 @@
       <c r="W27" s="3"/>
     </row>
     <row r="28" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="2" t="s">
         <v>109</v>
       </c>
@@ -1658,9 +1751,9 @@
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
     </row>
-    <row r="29" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+    <row r="29" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
         <v>110</v>
       </c>
@@ -1688,10 +1781,10 @@
       <c r="W29" s="3"/>
     </row>
     <row r="30" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1721,8 +1814,8 @@
       <c r="W30" s="3"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="2" t="s">
         <v>112</v>
       </c>
@@ -1750,8 +1843,8 @@
       <c r="W31" s="3"/>
     </row>
     <row r="32" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="2" t="s">
         <v>113</v>
       </c>
@@ -1779,8 +1872,8 @@
       <c r="W32" s="3"/>
     </row>
     <row r="33" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="2" t="s">
         <v>114</v>
       </c>
@@ -1808,10 +1901,10 @@
       <c r="W33" s="3"/>
     </row>
     <row r="34" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1840,9 +1933,9 @@
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
     </row>
-    <row r="35" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+    <row r="35" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="2" t="s">
         <v>116</v>
       </c>
@@ -1869,9 +1962,9 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
     </row>
-    <row r="36" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+    <row r="36" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="2" t="s">
         <v>117</v>
       </c>
@@ -1898,9 +1991,9 @@
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
     </row>
-    <row r="37" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+    <row r="37" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="2" t="s">
         <v>118</v>
       </c>
@@ -1928,10 +2021,10 @@
       <c r="W37" s="3"/>
     </row>
     <row r="38" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1960,9 +2053,9 @@
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
     </row>
-    <row r="39" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+    <row r="39" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="2" t="s">
         <v>120</v>
       </c>
@@ -1990,8 +2083,8 @@
       <c r="W39" s="3"/>
     </row>
     <row r="40" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="2" t="s">
         <v>121</v>
       </c>
@@ -2018,9 +2111,9 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+    <row r="41" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="2" t="s">
         <v>122</v>
       </c>
@@ -2048,10 +2141,10 @@
       <c r="W41" s="3"/>
     </row>
     <row r="42" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -2081,8 +2174,8 @@
       <c r="W42" s="3"/>
     </row>
     <row r="43" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="2" t="s">
         <v>112</v>
       </c>
@@ -2109,9 +2202,9 @@
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
     </row>
-    <row r="44" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+    <row r="44" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="2" t="s">
         <v>124</v>
       </c>
@@ -2138,9 +2231,9 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
-    <row r="45" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+    <row r="45" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="2" t="s">
         <v>125</v>
       </c>
@@ -2168,10 +2261,10 @@
       <c r="W45" s="3"/>
     </row>
     <row r="46" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -2200,9 +2293,9 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
     </row>
-    <row r="47" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+    <row r="47" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="2" t="s">
         <v>127</v>
       </c>
@@ -2229,9 +2322,9 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+    <row r="48" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
       <c r="C48" s="2" t="s">
         <v>128</v>
       </c>
@@ -2258,9 +2351,9 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+    <row r="49" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
       <c r="C49" s="2" t="s">
         <v>129</v>
       </c>
@@ -2287,11 +2380,11 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -2321,8 +2414,8 @@
       <c r="W50" s="3"/>
     </row>
     <row r="51" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
       <c r="C51" s="2" t="s">
         <v>24</v>
       </c>
@@ -2349,9 +2442,9 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+    <row r="52" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
       <c r="C52" s="2" t="s">
         <v>25</v>
       </c>
@@ -2378,9 +2471,9 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
     </row>
-    <row r="53" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
+    <row r="53" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
       <c r="C53" s="2" t="s">
         <v>26</v>
       </c>
@@ -2409,10 +2502,10 @@
       <c r="X53" s="3"/>
     </row>
     <row r="54" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -2443,8 +2536,8 @@
       <c r="X54" s="3"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
         <v>29</v>
       </c>
@@ -2473,8 +2566,8 @@
       <c r="X55" s="3"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
       <c r="C56" s="3" t="s">
         <v>30</v>
       </c>
@@ -2503,8 +2596,8 @@
       <c r="X56" s="3"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
       <c r="C57" s="3" t="s">
         <v>31</v>
       </c>
@@ -2533,10 +2626,10 @@
       <c r="X57" s="3"/>
     </row>
     <row r="58" spans="1:24" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2567,8 +2660,8 @@
       <c r="X58" s="3"/>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
       <c r="C59" s="3" t="s">
         <v>34</v>
       </c>
@@ -2597,8 +2690,8 @@
       <c r="X59" s="3"/>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
       <c r="C60" s="3" t="s">
         <v>35</v>
       </c>
@@ -2627,8 +2720,8 @@
       <c r="X60" s="3"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="3" t="s">
         <v>36</v>
       </c>
@@ -2657,10 +2750,10 @@
       <c r="X61" s="3"/>
     </row>
     <row r="62" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -2690,9 +2783,9 @@
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
     </row>
-    <row r="63" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="3" t="s">
         <v>39</v>
       </c>
@@ -2720,9 +2813,9 @@
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
     </row>
-    <row r="64" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="3" t="s">
         <v>40</v>
       </c>
@@ -2751,8 +2844,8 @@
       <c r="X64" s="3"/>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="3" t="s">
         <v>41</v>
       </c>
@@ -2781,10 +2874,10 @@
       <c r="X65" s="3"/>
     </row>
     <row r="66" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -2814,9 +2907,9 @@
       <c r="W66" s="3"/>
       <c r="X66" s="3"/>
     </row>
-    <row r="67" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
       <c r="C67" s="3" t="s">
         <v>44</v>
       </c>
@@ -2844,9 +2937,9 @@
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
     </row>
-    <row r="68" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="3" t="s">
         <v>45</v>
       </c>
@@ -2874,9 +2967,9 @@
       <c r="W68" s="3"/>
       <c r="X68" s="3"/>
     </row>
-    <row r="69" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="3" t="s">
         <v>46</v>
       </c>
@@ -2905,10 +2998,10 @@
       <c r="X69" s="3"/>
     </row>
     <row r="70" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -2938,9 +3031,9 @@
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
     </row>
-    <row r="71" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
       <c r="C71" s="3" t="s">
         <v>49</v>
       </c>
@@ -2969,8 +3062,8 @@
       <c r="X71" s="3"/>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
         <v>50</v>
       </c>
@@ -2998,9 +3091,9 @@
       <c r="W72" s="3"/>
       <c r="X72" s="3"/>
     </row>
-    <row r="73" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
       <c r="C73" s="3" t="s">
         <v>51</v>
       </c>
@@ -3029,10 +3122,10 @@
       <c r="X73" s="3"/>
     </row>
     <row r="74" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -3062,9 +3155,9 @@
       <c r="W74" s="3"/>
       <c r="X74" s="3"/>
     </row>
-    <row r="75" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
       <c r="C75" s="3" t="s">
         <v>55</v>
       </c>
@@ -3093,8 +3186,8 @@
       <c r="X75" s="3"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
       <c r="C76" s="3" t="s">
         <v>56</v>
       </c>
@@ -3122,9 +3215,9 @@
       <c r="W76" s="3"/>
       <c r="X76" s="3"/>
     </row>
-    <row r="77" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+    <row r="77" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
       <c r="C77" s="3" t="s">
         <v>57</v>
       </c>
@@ -3153,10 +3246,10 @@
       <c r="X77" s="3"/>
     </row>
     <row r="78" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -3187,8 +3280,8 @@
       <c r="X78" s="3"/>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
       <c r="C79" s="3" t="s">
         <v>60</v>
       </c>
@@ -3217,8 +3310,8 @@
       <c r="X79" s="3"/>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
       <c r="C80" s="3" t="s">
         <v>61</v>
       </c>
@@ -3247,8 +3340,8 @@
       <c r="X80" s="3"/>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
         <v>62</v>
       </c>
@@ -3276,11 +3369,11 @@
       <c r="W81" s="3"/>
       <c r="X81" s="3"/>
     </row>
-    <row r="82" spans="1:24" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="82" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -3310,9 +3403,9 @@
       <c r="W82" s="3"/>
       <c r="X82" s="3"/>
     </row>
-    <row r="83" spans="1:24" ht="120" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+    <row r="83" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
       <c r="C83" s="3" t="s">
         <v>65</v>
       </c>
@@ -3340,9 +3433,9 @@
       <c r="W83" s="3"/>
       <c r="X83" s="3"/>
     </row>
-    <row r="84" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+    <row r="84" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
         <v>66</v>
       </c>
@@ -3370,9 +3463,9 @@
       <c r="W84" s="3"/>
       <c r="X84" s="3"/>
     </row>
-    <row r="85" spans="1:24" ht="75" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+    <row r="85" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
         <v>67</v>
       </c>
@@ -3401,10 +3494,10 @@
       <c r="X85" s="3"/>
     </row>
     <row r="86" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -3434,9 +3527,9 @@
       <c r="W86" s="3"/>
       <c r="X86" s="3"/>
     </row>
-    <row r="87" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
         <v>70</v>
       </c>
@@ -3464,9 +3557,9 @@
       <c r="W87" s="3"/>
       <c r="X87" s="3"/>
     </row>
-    <row r="88" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
         <v>71</v>
       </c>
@@ -3494,9 +3587,9 @@
       <c r="W88" s="3"/>
       <c r="X88" s="3"/>
     </row>
-    <row r="89" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
         <v>72</v>
       </c>
@@ -3524,11 +3617,11 @@
       <c r="W89" s="3"/>
       <c r="X89" s="3"/>
     </row>
-    <row r="90" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -3558,9 +3651,9 @@
       <c r="W90" s="3"/>
       <c r="X90" s="3"/>
     </row>
-    <row r="91" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+    <row r="91" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
       <c r="C91" s="3" t="s">
         <v>75</v>
       </c>
@@ -3588,9 +3681,9 @@
       <c r="W91" s="3"/>
       <c r="X91" s="3"/>
     </row>
-    <row r="92" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
       <c r="C92" s="3" t="s">
         <v>76</v>
       </c>
@@ -3619,8 +3712,8 @@
       <c r="X92" s="3"/>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
       <c r="C93" s="3" t="s">
         <v>77</v>
       </c>
@@ -3649,10 +3742,10 @@
       <c r="X93" s="3"/>
     </row>
     <row r="94" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -3683,8 +3776,8 @@
       <c r="X94" s="3"/>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
       <c r="C95" s="3" t="s">
         <v>80</v>
       </c>
@@ -3713,8 +3806,8 @@
       <c r="X95" s="3"/>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
       <c r="C96" s="3" t="s">
         <v>81</v>
       </c>
@@ -3743,8 +3836,8 @@
       <c r="X96" s="3"/>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
       <c r="C97" s="3" t="s">
         <v>82</v>
       </c>
@@ -3772,11 +3865,19 @@
       <c r="W97" s="3"/>
       <c r="X97" s="3"/>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+    <row r="98" spans="1:24" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
@@ -3799,10 +3900,14 @@
       <c r="X98" s="3"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
@@ -3825,10 +3930,14 @@
       <c r="X99" s="3"/>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
@@ -3851,10 +3960,14 @@
       <c r="X100" s="3"/>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
@@ -3876,11 +3989,19 @@
       <c r="W101" s="3"/>
       <c r="X101" s="3"/>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+    <row r="102" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
@@ -3903,10 +4024,14 @@
       <c r="X102" s="3"/>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
@@ -3929,10 +4054,14 @@
       <c r="X103" s="3"/>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
@@ -3955,10 +4084,14 @@
       <c r="X104" s="3"/>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -3980,11 +4113,19 @@
       <c r="W105" s="3"/>
       <c r="X105" s="3"/>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
+    <row r="106" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -4007,10 +4148,14 @@
       <c r="X106" s="3"/>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -4033,10 +4178,14 @@
       <c r="X107" s="3"/>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A108" s="3"/>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
@@ -4059,10 +4208,14 @@
       <c r="X108" s="3"/>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -4084,11 +4237,19 @@
       <c r="W109" s="3"/>
       <c r="X109" s="3"/>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+    <row r="110" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -4111,10 +4272,14 @@
       <c r="X110" s="3"/>
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A111" s="3"/>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
@@ -4137,10 +4302,14 @@
       <c r="X111" s="3"/>
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A112" s="3"/>
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
@@ -4163,10 +4332,14 @@
       <c r="X112" s="3"/>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -4188,11 +4361,19 @@
       <c r="W113" s="3"/>
       <c r="X113" s="3"/>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A114" s="3"/>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+    <row r="114" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
@@ -4215,10 +4396,14 @@
       <c r="X114" s="3"/>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
@@ -4241,10 +4426,14 @@
       <c r="X115" s="3"/>
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
@@ -4267,10 +4456,14 @@
       <c r="X116" s="3"/>
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
@@ -4292,11 +4485,19 @@
       <c r="W117" s="3"/>
       <c r="X117" s="3"/>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+    <row r="118" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
@@ -4319,10 +4520,14 @@
       <c r="X118" s="3"/>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
@@ -4345,10 +4550,14 @@
       <c r="X119" s="3"/>
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
@@ -4371,10 +4580,14 @@
       <c r="X120" s="3"/>
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -5437,55 +5650,67 @@
       <c r="X161" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="60">
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="B110:B113"/>
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="B114:B117"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="B78:B81"/>
     <mergeCell ref="A86:A89"/>
     <mergeCell ref="B86:B89"/>
     <mergeCell ref="A90:A93"/>
     <mergeCell ref="B90:B93"/>
     <mergeCell ref="A94:A97"/>
     <mergeCell ref="B94:B97"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
creacion del archivo y corte de control
</commit_message>
<xml_diff>
--- a/Preguntas y respuestas.xlsx
+++ b/Preguntas y respuestas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\Facultad 2019\Algoritmos y estructura de datos\TP 2019\Repositorio\TPAlgoritmos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1970716-2EAE-408A-8D0D-409DFFD6BD4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79042E04-C797-4D0B-BD4D-336859977EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{568DC9B8-9665-4EC8-9CD9-1389A254C195}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{568DC9B8-9665-4EC8-9CD9-1389A254C195}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>¿En qué frontera se encuentra el Monte Everest?</t>
   </si>
   <si>
-    <t>¿Cuál es el desierto más grande?</t>
-  </si>
-  <si>
     <t>¿Dónde se encuentra el Gran Cañón?</t>
   </si>
   <si>
@@ -607,6 +604,9 @@
   </si>
   <si>
     <t>D-Nahasaapematilon</t>
+  </si>
+  <si>
+    <t>¿Cuál es el desierto cálido más grande?</t>
   </si>
 </sst>
 </file>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC6222F-3F2B-43BB-8383-758C7F06C17A}">
   <dimension ref="A1:X161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -1070,7 +1070,7 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -1099,7 +1099,7 @@
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1128,7 +1128,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -1161,7 +1161,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -1190,7 +1190,7 @@
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -1219,7 +1219,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -1248,7 +1248,7 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -1281,7 +1281,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
@@ -1310,7 +1310,7 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -1339,7 +1339,7 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -1368,7 +1368,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -1401,7 +1401,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
@@ -1430,7 +1430,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
@@ -1459,7 +1459,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -1488,7 +1488,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -1521,7 +1521,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
@@ -1550,7 +1550,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1579,7 +1579,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -1608,7 +1608,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -1641,7 +1641,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -1670,7 +1670,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
@@ -1699,7 +1699,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>7</v>
@@ -1728,7 +1728,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
@@ -1761,7 +1761,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1790,7 +1790,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
@@ -1819,7 +1819,7 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>7</v>
@@ -1848,7 +1848,7 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1881,7 +1881,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>7</v>
@@ -1910,7 +1910,7 @@
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -1939,7 +1939,7 @@
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
@@ -1968,7 +1968,7 @@
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
@@ -2001,7 +2001,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
@@ -2030,7 +2030,7 @@
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
@@ -2059,7 +2059,7 @@
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>7</v>
@@ -2088,7 +2088,7 @@
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>6</v>
@@ -2118,10 +2118,10 @@
         <v>13</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
@@ -2150,7 +2150,7 @@
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -2179,10 +2179,10 @@
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2208,10 +2208,10 @@
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2238,10 +2238,10 @@
         <v>13</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
@@ -2270,7 +2270,7 @@
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
@@ -2299,7 +2299,7 @@
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>7</v>
@@ -2328,7 +2328,7 @@
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
@@ -2358,10 +2358,10 @@
         <v>16</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
@@ -2390,7 +2390,7 @@
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
@@ -2419,7 +2419,7 @@
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>7</v>
@@ -2448,7 +2448,7 @@
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -2475,13 +2475,13 @@
     </row>
     <row r="50" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="C50" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>7</v>
@@ -2510,7 +2510,7 @@
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>6</v>
@@ -2539,7 +2539,7 @@
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
@@ -2568,7 +2568,7 @@
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="54" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>6</v>
@@ -2632,7 +2632,7 @@
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>6</v>
@@ -2662,7 +2662,7 @@
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>7</v>
@@ -2692,7 +2692,7 @@
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>6</v>
@@ -2720,13 +2720,13 @@
     </row>
     <row r="58" spans="1:24" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>7</v>
@@ -2756,7 +2756,7 @@
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>6</v>
@@ -2786,7 +2786,7 @@
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>6</v>
@@ -2816,7 +2816,7 @@
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>6</v>
@@ -2844,13 +2844,13 @@
     </row>
     <row r="62" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>6</v>
@@ -2880,7 +2880,7 @@
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>7</v>
@@ -2910,7 +2910,7 @@
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>6</v>
@@ -2940,7 +2940,7 @@
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>6</v>
@@ -2968,13 +2968,13 @@
     </row>
     <row r="66" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>6</v>
@@ -3004,7 +3004,7 @@
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>6</v>
@@ -3034,7 +3034,7 @@
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>6</v>
@@ -3064,7 +3064,7 @@
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>7</v>
@@ -3092,13 +3092,13 @@
     </row>
     <row r="70" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>7</v>
@@ -3128,7 +3128,7 @@
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>6</v>
@@ -3158,7 +3158,7 @@
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>6</v>
@@ -3188,7 +3188,7 @@
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>6</v>
@@ -3216,13 +3216,13 @@
     </row>
     <row r="74" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>6</v>
@@ -3252,7 +3252,7 @@
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>6</v>
@@ -3282,7 +3282,7 @@
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>7</v>
@@ -3312,7 +3312,7 @@
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>6</v>
@@ -3340,13 +3340,13 @@
     </row>
     <row r="78" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>7</v>
@@ -3376,7 +3376,7 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>6</v>
@@ -3406,7 +3406,7 @@
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>6</v>
@@ -3436,7 +3436,7 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>6</v>
@@ -3464,13 +3464,13 @@
     </row>
     <row r="82" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>6</v>
@@ -3500,7 +3500,7 @@
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>7</v>
@@ -3530,7 +3530,7 @@
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>6</v>
@@ -3560,7 +3560,7 @@
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>6</v>
@@ -3588,13 +3588,13 @@
     </row>
     <row r="86" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>6</v>
@@ -3624,7 +3624,7 @@
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>7</v>
@@ -3654,7 +3654,7 @@
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>6</v>
@@ -3684,7 +3684,7 @@
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>6</v>
@@ -3712,13 +3712,13 @@
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B90" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>6</v>
@@ -3748,7 +3748,7 @@
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>6</v>
@@ -3778,7 +3778,7 @@
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>6</v>
@@ -3808,7 +3808,7 @@
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>7</v>
@@ -3836,13 +3836,13 @@
     </row>
     <row r="94" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>7</v>
@@ -3872,7 +3872,7 @@
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>6</v>
@@ -3902,7 +3902,7 @@
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>6</v>
@@ -3932,7 +3932,7 @@
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>6</v>
@@ -3960,13 +3960,13 @@
     </row>
     <row r="98" spans="1:24" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="C98" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>6</v>
@@ -3996,7 +3996,7 @@
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>7</v>
@@ -4026,7 +4026,7 @@
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>6</v>
@@ -4056,7 +4056,7 @@
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>6</v>
@@ -4084,13 +4084,13 @@
     </row>
     <row r="102" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B102" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>6</v>
@@ -4120,7 +4120,7 @@
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>6</v>
@@ -4150,7 +4150,7 @@
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>7</v>
@@ -4180,7 +4180,7 @@
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>6</v>
@@ -4208,13 +4208,13 @@
     </row>
     <row r="106" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B106" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>6</v>
@@ -4244,7 +4244,7 @@
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>7</v>
@@ -4274,7 +4274,7 @@
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>6</v>
@@ -4304,7 +4304,7 @@
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>6</v>
@@ -4332,13 +4332,13 @@
     </row>
     <row r="110" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B110" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>7</v>
@@ -4368,7 +4368,7 @@
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>6</v>
@@ -4398,7 +4398,7 @@
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>6</v>
@@ -4428,7 +4428,7 @@
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>6</v>
@@ -4456,13 +4456,13 @@
     </row>
     <row r="114" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B114" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>7</v>
@@ -4492,7 +4492,7 @@
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>6</v>
@@ -4522,7 +4522,7 @@
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>6</v>
@@ -4552,7 +4552,7 @@
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>6</v>
@@ -4580,13 +4580,13 @@
     </row>
     <row r="118" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B118" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>6</v>
@@ -4616,7 +4616,7 @@
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>6</v>
@@ -4646,7 +4646,7 @@
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>7</v>
@@ -4676,7 +4676,7 @@
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>6</v>
@@ -4704,13 +4704,13 @@
     </row>
     <row r="122" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="C122" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>7</v>
@@ -4740,7 +4740,7 @@
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>6</v>
@@ -4770,7 +4770,7 @@
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>6</v>
@@ -4800,7 +4800,7 @@
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>6</v>
@@ -4828,13 +4828,13 @@
     </row>
     <row r="126" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B126" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>6</v>
@@ -4864,7 +4864,7 @@
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>6</v>
@@ -4894,7 +4894,7 @@
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>6</v>
@@ -4924,7 +4924,7 @@
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>7</v>
@@ -4952,13 +4952,13 @@
     </row>
     <row r="130" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>6</v>
@@ -4988,7 +4988,7 @@
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>6</v>
@@ -5018,7 +5018,7 @@
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>6</v>
@@ -5048,7 +5048,7 @@
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>7</v>
@@ -5076,13 +5076,13 @@
     </row>
     <row r="134" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>6</v>
@@ -5112,7 +5112,7 @@
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>7</v>
@@ -5142,7 +5142,7 @@
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>6</v>
@@ -5172,7 +5172,7 @@
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>6</v>
@@ -5200,13 +5200,13 @@
     </row>
     <row r="138" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B138" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>7</v>
@@ -5236,7 +5236,7 @@
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>6</v>
@@ -5266,7 +5266,7 @@
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>6</v>
@@ -5296,7 +5296,7 @@
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>6</v>
@@ -5324,13 +5324,13 @@
     </row>
     <row r="142" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>6</v>
@@ -5360,7 +5360,7 @@
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>6</v>
@@ -5390,7 +5390,7 @@
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>7</v>
@@ -5420,7 +5420,7 @@
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>6</v>
@@ -5864,78 +5864,78 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="B110:B113"/>
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="B114:B117"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="A122:A125"/>
+    <mergeCell ref="B122:B125"/>
+    <mergeCell ref="A126:A129"/>
+    <mergeCell ref="B126:B129"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="B130:B133"/>
     <mergeCell ref="A134:A137"/>
     <mergeCell ref="B134:B137"/>
     <mergeCell ref="A138:A141"/>
     <mergeCell ref="B138:B141"/>
     <mergeCell ref="A142:A145"/>
     <mergeCell ref="B142:B145"/>
-    <mergeCell ref="A122:A125"/>
-    <mergeCell ref="B122:B125"/>
-    <mergeCell ref="A126:A129"/>
-    <mergeCell ref="B126:B129"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="B130:B133"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A98:A101"/>
-    <mergeCell ref="B98:B101"/>
-    <mergeCell ref="A102:A105"/>
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="B106:B109"/>
-    <mergeCell ref="A110:A113"/>
-    <mergeCell ref="B110:B113"/>
-    <mergeCell ref="A114:A117"/>
-    <mergeCell ref="B114:B117"/>
-    <mergeCell ref="A118:A121"/>
-    <mergeCell ref="B118:B121"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>